<commit_message>
I need to look at an alt solution
</commit_message>
<xml_diff>
--- a/CH-074 Determining missing fields.xlsx
+++ b/CH-074 Determining missing fields.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8B4920-D1A2-4BA0-9A63-E8751E5BCEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B6558B-94C0-4441-8D02-019A32EE0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="720" windowWidth="23016" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37470" yWindow="930" windowWidth="28800" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="Alt" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$B$2:$B$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,8 +42,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
   <si>
     <t>Question</t>
   </si>
@@ -117,6 +143,9 @@
   </si>
   <si>
     <t>Record No</t>
+  </si>
+  <si>
+    <t>Phone, Website</t>
   </si>
 </sst>
 </file>
@@ -576,15 +605,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:colOff>21591</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>84455</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1906</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -599,8 +628,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3280411" y="1617345"/>
-          <a:ext cx="4295775" cy="3206115"/>
+          <a:off x="3279141" y="1627505"/>
+          <a:ext cx="4291965" cy="3579495"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -942,12 +971,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="1327" row="9">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{14731FE8-8975-4DB9-B4D7-361E499E3962}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1209,4 +1265,601 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90A6E8B-8F26-4DBF-937C-3D2460F871BC}">
+  <dimension ref="B1:L28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="F1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9673FE-4A7C-48AB-A742-CC482FD8F8CD}">
+  <dimension ref="B1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24"/>
+      <c r="F1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="9"/>
+      <c r="F20" s="6" t="str" cm="1">
+        <f t="array" ref="F20:H24">_xlfn.LET(
+    _xlpm.b, B3:B15,
+    _xlpm.m, _xlfn.MAP(_xlpm.b, _xlfn.LAMBDA(_xlpm.b, COUNTIF(B3:_xlpm.b, "Name"))),
+    _xlfn.REDUCE(
+        F2:H2,
+        _xlfn.UNIQUE(_xlpm.m),
+        _xlfn.LAMBDA(_xlpm.i,_xlpm.x,
+            _xlfn.LET(
+                _xlpm.e, _xlfn.UNIQUE(_xlpm.b),
+                _xlpm.f, _xlfn._xlws.FILTER(_xlpm.b, _xlpm.m = _xlpm.x),
+                _xlfn.VSTACK(
+                    _xlpm.i,
+                    _xlfn.HSTACK(
+                        _xlpm.x,
+                        _xlfn.BYCOL(
+                            IF(MMULT(N(_xlfn.TOROW(_xlpm.f) = _xlpm.e), _xlfn.SEQUENCE(ROWS(_xlpm.f)) ^ 0) = {0,2}, _xlpm.e, ""),
+                            _xlfn.LAMBDA(_xlpm.c, _xlfn.TEXTJOIN(", ", , _xlpm.c))
+                        )
+                    )
+                )
+            )
+        )
+    )
+)</f>
+        <v>Record No</v>
+      </c>
+      <c r="G20" t="str">
+        <v>Missing Fields</v>
+      </c>
+      <c r="H20" t="str">
+        <v>Duplicate fields</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+      <c r="H21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+      <c r="F22" s="6">
+        <v>2</v>
+      </c>
+      <c r="G22" t="str">
+        <v/>
+      </c>
+      <c r="H22" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="23" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="9"/>
+      <c r="F23" s="6">
+        <v>3</v>
+      </c>
+      <c r="G23" t="str">
+        <v>Phone, Website</v>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="10"/>
+      <c r="F24" s="6">
+        <v>4</v>
+      </c>
+      <c r="G24" t="str">
+        <v>Family, Phone</v>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tearing apart the alternate
</commit_message>
<xml_diff>
--- a/CH-074 Determining missing fields.xlsx
+++ b/CH-074 Determining missing fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B6558B-94C0-4441-8D02-019A32EE0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C086D6AE-2A3D-4DD2-B68F-ADF973876C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-37470" yWindow="930" windowWidth="28800" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,7 +985,9 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{7BE8176E-25CC-43F8-86A0-64D8EFCAC463}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
@@ -1533,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9673FE-4A7C-48AB-A742-CC482FD8F8CD}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1749,16 +1751,16 @@
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E20" s="9"/>
       <c r="F20" s="6" t="str" cm="1">
         <f t="array" ref="F20:H24">_xlfn.LET(
@@ -1793,8 +1795,12 @@
       <c r="H20" t="str">
         <v>Duplicate fields</v>
       </c>
-    </row>
-    <row r="21" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J20" cm="1">
+        <f t="array" ref="J20:J32">_xlfn.LET(_xlpm.b, B3:B15, _xlpm.m, _xlfn.MAP(_xlpm.b, _xlfn.LAMBDA(_xlpm.b, COUNTIF(B3:_xlpm.b, "Name"))), _xlpm.m)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E21" s="9"/>
       <c r="F21" s="6">
         <v>1</v>
@@ -1805,8 +1811,11 @@
       <c r="H21" t="str">
         <v/>
       </c>
-    </row>
-    <row r="22" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E22" s="9"/>
       <c r="F22" s="6">
         <v>2</v>
@@ -1817,8 +1826,11 @@
       <c r="H22" t="str">
         <v>Phone</v>
       </c>
-    </row>
-    <row r="23" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E23" s="9"/>
       <c r="F23" s="6">
         <v>3</v>
@@ -1829,8 +1841,11 @@
       <c r="H23" t="str">
         <v/>
       </c>
-    </row>
-    <row r="24" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E24" s="10"/>
       <c r="F24" s="6">
         <v>4</v>
@@ -1841,18 +1856,53 @@
       <c r="H24" t="str">
         <v/>
       </c>
-    </row>
-    <row r="25" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E28" s="10"/>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="J30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="J31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="J32">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1862,4 +1912,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BE8176E-25CC-43F8-86A0-64D8EFCAC463}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Completed my EDA. I now understand what is going on
</commit_message>
<xml_diff>
--- a/CH-074 Determining missing fields.xlsx
+++ b/CH-074 Determining missing fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C086D6AE-2A3D-4DD2-B68F-ADF973876C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88B4B48-7D65-427C-9F9F-DE1DEA2D13B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37470" yWindow="930" windowWidth="28800" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19960" yWindow="4260" windowWidth="19240" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="30">
   <si>
     <t>Question</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>Phone, Website</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>Row</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +256,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -299,12 +320,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -367,9 +441,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -973,7 +1055,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="1327" row="9">
+  <wetp:taskpane dockstate="right" visibility="0" width="1173" row="9">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -991,6 +1073,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1021,15 +1106,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="F1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -1271,10 +1356,554 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90A6E8B-8F26-4DBF-937C-3D2460F871BC}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="2" cm="1">
+        <f t="array" ref="O5:O8">MMULT(_xlfn.ANCHORARRAY(I12),_xlfn.ANCHORARRAY(N12))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="2" t="str" cm="1">
+        <f t="array" ref="J6:J9">_xlfn.UNIQUE(B3:B15)</f>
+        <v>Name</v>
+      </c>
+      <c r="O6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="J7" s="2" t="str">
+        <v>Family</v>
+      </c>
+      <c r="O7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="G8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9"/>
+      <c r="G9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9" t="str">
+        <v>Website</v>
+      </c>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12:H16">_xlfn._xlws.FILTER(B3:B15,_xlfn.ANCHORARRAY(F18)=H9)</f>
+        <v>Name</v>
+      </c>
+      <c r="I12" s="25" cm="1">
+        <f t="array" ref="I12:M15">_xlfn.IFNA(N(_xlfn.TOROW(_xlfn.ANCHORARRAY(H12))=J6:J9),0)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="25">
+        <v>0</v>
+      </c>
+      <c r="K12" s="25">
+        <v>0</v>
+      </c>
+      <c r="L12" s="25">
+        <v>0</v>
+      </c>
+      <c r="M12" s="25">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24" cm="1">
+        <f t="array" ref="N12:N16">_xlfn.SEQUENCE(ROWS(_xlfn.ANCHORARRAY(H12)))^0</f>
+        <v>1</v>
+      </c>
+      <c r="O12" t="b" cm="1">
+        <f t="array" ref="O12:P15">MMULT(_xlfn.ANCHORARRAY(I12),_xlfn.ANCHORARRAY(N12))={0,2}</f>
+        <v>0</v>
+      </c>
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="27" t="str" cm="1">
+        <f t="array" ref="Q12:R15">IF(_xlfn.ANCHORARRAY(O12),_xlfn.ANCHORARRAY(J6),"")</f>
+        <v/>
+      </c>
+      <c r="R12" s="27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="H13" t="str">
+        <v>Family</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0</v>
+      </c>
+      <c r="J13" s="25">
+        <v>1</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0</v>
+      </c>
+      <c r="N13" s="24">
+        <v>1</v>
+      </c>
+      <c r="O13" t="b">
+        <v>0</v>
+      </c>
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="27" t="str">
+        <v/>
+      </c>
+      <c r="R13" s="27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="H14" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25">
+        <v>0</v>
+      </c>
+      <c r="K14" s="25">
+        <v>1</v>
+      </c>
+      <c r="L14" s="25">
+        <v>1</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24">
+        <v>1</v>
+      </c>
+      <c r="O14" t="b">
+        <v>0</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="27" t="str">
+        <v/>
+      </c>
+      <c r="R14" s="27" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="H15" t="str">
+        <v>Phone</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0</v>
+      </c>
+      <c r="J15" s="25">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="25">
+        <v>0</v>
+      </c>
+      <c r="M15" s="25">
+        <v>1</v>
+      </c>
+      <c r="N15" s="24">
+        <v>1</v>
+      </c>
+      <c r="O15" t="b">
+        <v>0</v>
+      </c>
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="27" t="str">
+        <v/>
+      </c>
+      <c r="R15" s="27" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9"/>
+      <c r="H16" t="str">
+        <v>Website</v>
+      </c>
+      <c r="N16" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+      <c r="F18" cm="1">
+        <f t="array" ref="F18:F30">_xlfn.LET(_xlpm.b,B3:B15, _xlpm.m, _xlfn.MAP( _xlpm.b, _xlfn.LAMBDA(_xlpm.b, COUNTIF(B3:_xlpm.b, "Name"))), _xlpm.m)</f>
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" t="str">
+        <f>IF(H8=0,_xlfn.TEXTJOIN(",",TRUE,Q12:Q15),_xlfn.TEXTJOIN(",",TRUE,R12:R15))</f>
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="10"/>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="9"/>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="H20" s="29" t="str">
+        <f>I18</f>
+        <v>Phone</v>
+      </c>
+      <c r="I20" s="31">
+        <v>0</v>
+      </c>
+      <c r="J20" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="H21" s="30" cm="1">
+        <f t="array" ref="H21:H24">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(F18))</f>
+        <v>1</v>
+      </c>
+      <c r="I21" s="32" t="str">
+        <f t="dataTable" ref="I21:J24" dt2D="1" dtr="1" r1="H8" r2="H9"/>
+        <v/>
+      </c>
+      <c r="J21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="H22" s="30">
+        <v>2</v>
+      </c>
+      <c r="I22" s="32" t="str">
+        <v/>
+      </c>
+      <c r="J22" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="9"/>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="H23" s="30">
+        <v>3</v>
+      </c>
+      <c r="I23" s="32" t="str">
+        <v>Phone,Website</v>
+      </c>
+      <c r="J23" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="10"/>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="H24" s="30">
+        <v>4</v>
+      </c>
+      <c r="I24" s="32" t="str">
+        <v>Family,Phone</v>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+      <c r="F25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+      <c r="F26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+      <c r="F27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="10"/>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9673FE-4A7C-48AB-A742-CC482FD8F8CD}">
+  <dimension ref="B1:R32"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,18 +1918,18 @@
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="F1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
         <v>6</v>
       </c>
@@ -1317,8 +1946,12 @@
       <c r="H2" s="22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="R2" s="2" t="str" cm="1">
+        <f t="array" ref="R2:R5">_xlfn.UNIQUE(B3:B15)</f>
+        <v>Name</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
@@ -1333,8 +1966,11 @@
         <v>22</v>
       </c>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="R3" s="2" t="str">
+        <v>Family</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
@@ -1351,8 +1987,11 @@
       <c r="H4" s="15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="2" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
@@ -1369,8 +2008,11 @@
       <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="R5" s="2" t="str">
+        <v>Website</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +2030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>2</v>
       </c>
@@ -1396,8 +2038,24 @@
         <v>17</v>
       </c>
       <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="M7" s="2" cm="1">
+        <f t="array" ref="M7:P10">N(_xlfn.TOROW(K7:K10)=_xlfn.ANCHORARRAY(R2))</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
@@ -1408,10 +2066,24 @@
       <c r="E8"/>
       <c r="I8"/>
       <c r="J8"/>
-      <c r="K8"/>
+      <c r="K8" s="11" t="s">
+        <v>3</v>
+      </c>
       <c r="L8"/>
-    </row>
-    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
@@ -1422,10 +2094,24 @@
       <c r="E9"/>
       <c r="I9"/>
       <c r="J9"/>
-      <c r="K9"/>
+      <c r="K9" s="13" t="s">
+        <v>4</v>
+      </c>
       <c r="L9"/>
-    </row>
-    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="2">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>4</v>
       </c>
@@ -1436,10 +2122,24 @@
       <c r="E10"/>
       <c r="I10"/>
       <c r="J10"/>
-      <c r="K10"/>
+      <c r="K10" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="L10"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0</v>
+      </c>
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="14" t="s">
         <v>5</v>
       </c>
@@ -1448,7 +2148,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>2</v>
       </c>
@@ -1457,7 +2157,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>3</v>
       </c>
@@ -1465,8 +2165,29 @@
         <v>14</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J13" s="25" cm="1">
+        <f t="array" ref="J13:M16">N(_xlfn.TOROW(K7:K10) =_xlfn.ANCHORARRAY( R2))</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="25">
+        <v>0</v>
+      </c>
+      <c r="L13" s="25">
+        <v>0</v>
+      </c>
+      <c r="M13" s="25">
+        <v>0</v>
+      </c>
+      <c r="N13" s="24" cm="1">
+        <f t="array" ref="N13:N16">_xlfn.SEQUENCE(ROWS(K7:K10))^0</f>
+        <v>1</v>
+      </c>
+      <c r="P13" cm="1">
+        <f t="array" ref="P13:P16">MMULT(_xlfn.ANCHORARRAY(J13),_xlfn.ANCHORARRAY(N13))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="20" t="s">
         <v>2</v>
       </c>
@@ -1474,8 +2195,26 @@
         <v>19</v>
       </c>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J14" s="25">
+        <v>0</v>
+      </c>
+      <c r="K14" s="25">
+        <v>1</v>
+      </c>
+      <c r="L14" s="25">
+        <v>0</v>
+      </c>
+      <c r="M14" s="25">
+        <v>0</v>
+      </c>
+      <c r="N14" s="24">
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="20" t="s">
         <v>5</v>
       </c>
@@ -1483,273 +2222,45 @@
         <v>15</v>
       </c>
       <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J15" s="25">
+        <v>0</v>
+      </c>
+      <c r="K15" s="25">
+        <v>0</v>
+      </c>
+      <c r="L15" s="25">
+        <v>1</v>
+      </c>
+      <c r="M15" s="25">
+        <v>0</v>
+      </c>
+      <c r="N15" s="24">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E24" s="10"/>
-    </row>
-    <row r="25" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="5:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E28" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="F1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9673FE-4A7C-48AB-A742-CC482FD8F8CD}">
-  <dimension ref="B1:L32"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.44140625" customWidth="1"/>
-    <col min="5" max="5" width="4.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="F1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-    </row>
-    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="F2" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="F3" s="13">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5"/>
-      <c r="F4" s="16">
-        <v>2</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5"/>
-      <c r="F5" s="23">
-        <v>3</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="F6" s="20">
-        <v>4</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="5"/>
-      <c r="E8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-    </row>
-    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-    </row>
-    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10"/>
-      <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E16" s="9"/>
+      <c r="J16" s="25">
+        <v>0</v>
+      </c>
+      <c r="K16" s="25">
+        <v>0</v>
+      </c>
+      <c r="L16" s="25">
+        <v>0</v>
+      </c>
+      <c r="M16" s="25">
+        <v>1</v>
+      </c>
+      <c r="N16" s="24">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="5:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>

</xml_diff>

<commit_message>
Completed my version of the Alt function. Very good exercise.
</commit_message>
<xml_diff>
--- a/CH-074 Determining missing fields.xlsx
+++ b/CH-074 Determining missing fields.xlsx
@@ -8,18 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88B4B48-7D65-427C-9F9F-DE1DEA2D13B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C315E03-C540-4680-875E-32E4724462A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19960" yWindow="4260" windowWidth="19240" windowHeight="15410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19490" yWindow="100" windowWidth="19240" windowHeight="15410" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37120" yWindow="1280" windowWidth="19240" windowHeight="15410" activeTab="2" xr2:uid="{AD850033-FCBB-4CF2-86AD-BE64126B4E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt" sheetId="3" r:id="rId3"/>
+    <sheet name="MySingleFunction" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MySingleFunction!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="30">
   <si>
     <t>Question</t>
   </si>
@@ -443,15 +446,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1092,6 +1095,7 @@
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1106,15 +1110,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="F1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -1358,8 +1362,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90A6E8B-8F26-4DBF-937C-3D2460F871BC}">
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,15 +1384,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="F1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -1610,11 +1617,11 @@
       <c r="P12" t="b">
         <v>0</v>
       </c>
-      <c r="Q12" s="27" t="str" cm="1">
+      <c r="Q12" s="26" t="str" cm="1">
         <f t="array" ref="Q12:R15">IF(_xlfn.ANCHORARRAY(O12),_xlfn.ANCHORARRAY(J6),"")</f>
         <v/>
       </c>
-      <c r="R12" s="27" t="str">
+      <c r="R12" s="26" t="str">
         <v/>
       </c>
     </row>
@@ -1653,10 +1660,10 @@
       <c r="P13" t="b">
         <v>0</v>
       </c>
-      <c r="Q13" s="27" t="str">
+      <c r="Q13" s="26" t="str">
         <v/>
       </c>
-      <c r="R13" s="27" t="str">
+      <c r="R13" s="26" t="str">
         <v/>
       </c>
     </row>
@@ -1695,10 +1702,10 @@
       <c r="P14" t="b">
         <v>1</v>
       </c>
-      <c r="Q14" s="27" t="str">
+      <c r="Q14" s="26" t="str">
         <v/>
       </c>
-      <c r="R14" s="27" t="str">
+      <c r="R14" s="26" t="str">
         <v>Phone</v>
       </c>
     </row>
@@ -1737,10 +1744,10 @@
       <c r="P15" t="b">
         <v>0</v>
       </c>
-      <c r="Q15" s="27" t="str">
+      <c r="Q15" s="26" t="str">
         <v/>
       </c>
-      <c r="R15" s="27" t="str">
+      <c r="R15" s="26" t="str">
         <v/>
       </c>
     </row>
@@ -1781,14 +1788,14 @@
       <c r="F20">
         <v>1</v>
       </c>
-      <c r="H20" s="29" t="str">
+      <c r="H20" s="28" t="str">
         <f>I18</f>
         <v>Phone</v>
       </c>
-      <c r="I20" s="31">
-        <v>0</v>
-      </c>
-      <c r="J20" s="28">
+      <c r="I20" s="30">
+        <v>0</v>
+      </c>
+      <c r="J20" s="27">
         <v>1</v>
       </c>
     </row>
@@ -1797,11 +1804,11 @@
       <c r="F21">
         <v>1</v>
       </c>
-      <c r="H21" s="30" cm="1">
+      <c r="H21" s="29" cm="1">
         <f t="array" ref="H21:H24">_xlfn.UNIQUE(_xlfn.ANCHORARRAY(F18))</f>
         <v>1</v>
       </c>
-      <c r="I21" s="32" t="str">
+      <c r="I21" s="31" t="str">
         <f t="dataTable" ref="I21:J24" dt2D="1" dtr="1" r1="H8" r2="H9"/>
         <v/>
       </c>
@@ -1814,10 +1821,10 @@
       <c r="F22">
         <v>2</v>
       </c>
-      <c r="H22" s="30">
-        <v>2</v>
-      </c>
-      <c r="I22" s="32" t="str">
+      <c r="H22" s="29">
+        <v>2</v>
+      </c>
+      <c r="I22" s="31" t="str">
         <v/>
       </c>
       <c r="J22" t="str">
@@ -1829,10 +1836,10 @@
       <c r="F23">
         <v>2</v>
       </c>
-      <c r="H23" s="30">
+      <c r="H23" s="29">
         <v>3</v>
       </c>
-      <c r="I23" s="32" t="str">
+      <c r="I23" s="31" t="str">
         <v>Phone,Website</v>
       </c>
       <c r="J23" t="str">
@@ -1844,10 +1851,10 @@
       <c r="F24">
         <v>2</v>
       </c>
-      <c r="H24" s="30">
+      <c r="H24" s="29">
         <v>4</v>
       </c>
-      <c r="I24" s="32" t="str">
+      <c r="I24" s="31" t="str">
         <v>Family,Phone</v>
       </c>
       <c r="J24" t="str">
@@ -1903,7 +1910,10 @@
   <dimension ref="B1:R32"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="J13" sqref="J13:N16"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,15 +1929,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:18" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="F1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="2:18" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B2" s="22" t="s">
@@ -2425,6 +2435,337 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA983FC-689D-4C6E-9528-57346F834798}">
+  <dimension ref="B1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="9"/>
+      <c r="G20" s="22" t="str" cm="1">
+        <f t="array" ref="G20:I24">_xlfn.LET(_xlpm.b,B3:B15,
+     _xlpm.f, _xlfn.UNIQUE(_xlpm.b),
+     _xlpm.i, _xlfn.DROP(_xlfn.REDUCE("",_xlpm.b,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,COUNTIF(B3:_xlpm.v,"Name")))),1),
+     _xlpm.x, _xlfn.UNIQUE(_xlpm.i),
+     _xlpm.d, _xlfn.REDUCE(F2:H2,_xlpm.x,
+              _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                     _xlfn.VSTACK(_xlpm.a,
+                            _xlfn.HSTACK( _xlpm.v,
+                                    _xlfn.LET(
+                                        _xlpm.fx, _xlfn._xlws.FILTER(_xlpm.b,_xlpm.i=_xlpm.v),
+                                        _xlfn.BYCOL(IF(MMULT(N(_xlfn.TOROW(_xlpm.fx)=_xlpm.f),_xlfn.SEQUENCE(ROWS(_xlpm.fx))^0)={0,2},_xlpm.f,""),_xlfn.LAMBDA(_xlpm.c,_xlfn.TEXTJOIN(", ",,_xlpm.c)))
+                                       )
+                                  )
+                            )
+                    )
+               ),
+     _xlpm.d
+)</f>
+        <v>Record No</v>
+      </c>
+      <c r="H20" s="22" t="str">
+        <v>Missing Fields</v>
+      </c>
+      <c r="I20" s="22" t="str">
+        <v>Duplicate fields</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="str">
+        <v/>
+      </c>
+      <c r="I21" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+      <c r="G22" s="16">
+        <v>2</v>
+      </c>
+      <c r="H22" s="15" t="str">
+        <v/>
+      </c>
+      <c r="I22" s="15" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="9"/>
+      <c r="G23" s="23">
+        <v>3</v>
+      </c>
+      <c r="H23" s="19" t="str">
+        <v>Phone, Website</v>
+      </c>
+      <c r="I23" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="10"/>
+      <c r="G24" s="20">
+        <v>4</v>
+      </c>
+      <c r="H24" s="21" t="str">
+        <v>Family, Phone</v>
+      </c>
+      <c r="I24" s="21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>

<commit_message>
Modified my version to handle issue with dupes have 3 or more
</commit_message>
<xml_diff>
--- a/CH-074 Determining missing fields.xlsx
+++ b/CH-074 Determining missing fields.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C315E03-C540-4680-875E-32E4724462A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9402EC7F-9A2E-4CE1-BA28-860B8727606A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19490" yWindow="100" windowWidth="19240" windowHeight="15410" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-37120" yWindow="1280" windowWidth="19240" windowHeight="15410" activeTab="2" xr2:uid="{AD850033-FCBB-4CF2-86AD-BE64126B4E11}"/>
+    <workbookView xWindow="-21120" yWindow="530" windowWidth="19240" windowHeight="15410" firstSheet="1" activeTab="4" xr2:uid="{AD850033-FCBB-4CF2-86AD-BE64126B4E11}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt" sheetId="3" r:id="rId3"/>
     <sheet name="MySingleFunction" sheetId="4" r:id="rId4"/>
+    <sheet name="MySingleFunction2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Alt!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">MySingleFunction!$B$2:$B$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">MySingleFunction2!$B$2:$B$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -68,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="33">
   <si>
     <t>Question</t>
   </si>
@@ -158,6 +159,15 @@
   </si>
   <si>
     <t>Row</t>
+  </si>
+  <si>
+    <t>Some weaknesses.</t>
+  </si>
+  <si>
+    <t>Will fail if something is duplicated three or more times.</t>
+  </si>
+  <si>
+    <t>This approach fixes the issue with dupes having more than 2.</t>
   </si>
 </sst>
 </file>
@@ -1092,10 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1362,11 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90A6E8B-8F26-4DBF-937C-3D2460F871BC}">
   <dimension ref="B1:R30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="O13" sqref="O12:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1521,7 +1525,7 @@
         <v>28</v>
       </c>
       <c r="H8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8"/>
       <c r="J8" t="str">
@@ -1611,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="O12" t="b" cm="1">
-        <f t="array" ref="O12:P15">MMULT(_xlfn.ANCHORARRAY(I12),_xlfn.ANCHORARRAY(N12))={0,2}</f>
+        <f t="array" ref="O12:P15">_xlfn.HSTACK(MMULT(_xlfn.ANCHORARRAY(I12),_xlfn.ANCHORARRAY(N12))=0,MMULT(_xlfn.ANCHORARRAY(I12),_xlfn.ANCHORARRAY(N12))&gt;1)</f>
         <v>0</v>
       </c>
       <c r="P12" t="b">
@@ -1909,11 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9673FE-4A7C-48AB-A742-CC482FD8F8CD}">
   <dimension ref="B1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:N16"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2439,11 +2440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DA983FC-689D-4C6E-9528-57346F834798}">
   <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2653,9 +2651,15 @@
         <v>15</v>
       </c>
       <c r="E15" s="8"/>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E16" s="9"/>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="9"/>
@@ -2766,6 +2770,337 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44E08B97-F077-4EC1-8FF9-1CF01B6CD29F}">
+  <dimension ref="B1:L28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.44140625" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="F1" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="F2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="F3" s="13">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="F4" s="16">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="F5" s="23">
+        <v>3</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="F6" s="20">
+        <v>4</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+    </row>
+    <row r="9" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+    </row>
+    <row r="10" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="G15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E19" s="10"/>
+    </row>
+    <row r="20" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="9"/>
+      <c r="G20" s="22" t="str" cm="1">
+        <f t="array" ref="G20:I24">_xlfn.LET(_xlpm.b,B3:B15,
+     _xlpm.f, _xlfn.UNIQUE(_xlpm.b),
+     _xlpm.i, _xlfn.DROP(_xlfn.REDUCE("",_xlpm.b,_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,COUNTIF(B3:_xlpm.v,"Name")))),1),
+     _xlpm.x, _xlfn.UNIQUE(_xlpm.i),
+     _xlpm.d, _xlfn.REDUCE(F2:H2,_xlpm.x,
+              _xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+                     _xlfn.VSTACK(_xlpm.a,
+                            _xlfn.HSTACK( _xlpm.v,
+                                    _xlfn.LET(
+                                        _xlpm.fx, _xlfn._xlws.FILTER(_xlpm.b,_xlpm.i=_xlpm.v),
+                                        _xlfn.BYCOL(_xlfn.LET(_xlpm.z,MMULT(N(_xlfn.TOROW(_xlpm.fx)=_xlpm.f),_xlfn.SEQUENCE(ROWS(_xlpm.fx))^0),_xlfn.HSTACK(IF(_xlpm.z=0,_xlpm.f,""),IF(_xlpm.z&gt;1,_xlpm.f,""))),_xlfn.LAMBDA(_xlpm.c,_xlfn.TEXTJOIN(", ",,_xlpm.c)))
+                                       )
+                                  )
+                            )
+                    )
+               ),
+     _xlpm.d
+)</f>
+        <v>Record No</v>
+      </c>
+      <c r="H20" s="22" t="str">
+        <v>Missing Fields</v>
+      </c>
+      <c r="I20" s="22" t="str">
+        <v>Duplicate fields</v>
+      </c>
+    </row>
+    <row r="21" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="12" t="str">
+        <v/>
+      </c>
+      <c r="I21" s="12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E22" s="9"/>
+      <c r="G22" s="16">
+        <v>2</v>
+      </c>
+      <c r="H22" s="15" t="str">
+        <v/>
+      </c>
+      <c r="I22" s="15" t="str">
+        <v>Phone</v>
+      </c>
+    </row>
+    <row r="23" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E23" s="9"/>
+      <c r="G23" s="23">
+        <v>3</v>
+      </c>
+      <c r="H23" s="19" t="str">
+        <v>Phone, Website</v>
+      </c>
+      <c r="I23" s="19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E24" s="10"/>
+      <c r="G24" s="20">
+        <v>4</v>
+      </c>
+      <c r="H24" s="21" t="str">
+        <v>Family, Phone</v>
+      </c>
+      <c r="I24" s="21" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E28" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
 </file>

</xml_diff>